<commit_message>
product excel and auth
</commit_message>
<xml_diff>
--- a/app/Imports/Excel/ProductsImport.xlsx
+++ b/app/Imports/Excel/ProductsImport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nield\KCLYNE-AdvWeb\app\Imports\EmployeeExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nield\test\KCLYNE-AdvWeb\app\Imports\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212B2FC8-91E6-44C5-B17C-5EBBF8CBE13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F224416-C432-42E7-8335-A6FBE46758ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="2415" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>RCB Shock 2.jpg,RCB Shock.png</t>
+  </si>
+  <si>
+    <t>Motul Oil 2.jpg,Motul Oil.jpg</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="330" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,6 +517,9 @@
       <c r="D2">
         <v>99</v>
       </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>